<commit_message>
Cambios 20170625_01 Finalizando observaciones
</commit_message>
<xml_diff>
--- a/requerimientos/observacion_20170624.xlsx
+++ b/requerimientos/observacion_20170624.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>errores desde la pagina de administracion</t>
   </si>
@@ -74,9 +74,6 @@
     <t>editar usuario</t>
   </si>
   <si>
-    <t>al editar un campo que no sea la contraseña y guardas la contraseña cambia tambien</t>
-  </si>
-  <si>
     <t>errores desde la pagina de usuario</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>SOLUCIONADO</t>
+  </si>
+  <si>
+    <t>al editar un campo que no sea la contraseña y guardas, la contraseña cambia tambien</t>
   </si>
 </sst>
 </file>
@@ -483,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +495,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -507,7 +507,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -529,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -545,7 +545,7 @@
         <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -556,7 +556,7 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -567,7 +567,7 @@
         <v>5</v>
       </c>
       <c r="K7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -578,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="K8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -589,7 +589,7 @@
         <v>7</v>
       </c>
       <c r="K9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -605,7 +605,7 @@
         <v>9</v>
       </c>
       <c r="K11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
         <v>10</v>
       </c>
       <c r="K12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>11</v>
       </c>
       <c r="K13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -642,6 +642,9 @@
       <c r="B15" t="s">
         <v>13</v>
       </c>
+      <c r="K15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -650,31 +653,40 @@
       <c r="B16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -686,145 +698,181 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="K23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="K25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" s="2" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="K29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="K31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="K34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="K35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="K37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
       <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="K38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="K41" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>